<commit_message>
ajout states pd concat
</commit_message>
<xml_diff>
--- a/data/col aide.xlsx
+++ b/data/col aide.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\SDA\Projet 4 - Classification\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5283624-856D-4929-B880-29839E7CB041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DCE3B1-6246-408C-9D3C-78F6EAF45496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2865" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{879FF251-0387-4E4C-B457-5003EFE58310}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{879FF251-0387-4E4C-B457-5003EFE58310}"/>
   </bookViews>
   <sheets>
     <sheet name="Col Pop_est" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="3" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="4" r:id="rId4"/>
+    <sheet name="Ajout du niveau ETAT" sheetId="5" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="3" r:id="rId4"/>
+    <sheet name="Feuil3" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Col Pop_est'!$B$1:$B$66</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="356">
   <si>
     <t>Deaths_2015</t>
   </si>
@@ -616,6 +617,498 @@
   </si>
   <si>
     <t>Rural-urban_Continuum Code_2013</t>
+  </si>
+  <si>
+    <t>FIPS Code</t>
+  </si>
+  <si>
+    <t>Area name</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>01000</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>02000</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>04000</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>05000</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>06000</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>08000</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>09000</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>11000</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>13000</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>16000</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>17000</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>18000</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>19000</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>21000</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>22000</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Lousiana</t>
+  </si>
+  <si>
+    <t>23000</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>24000</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>26000</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>27000</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>28000</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>29000</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>31000</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>32000</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>33000</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>34000</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>35000</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>36000</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>37000</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>38000</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>39000</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>40000</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>41000</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>42000</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>44000</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>45000</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>46000</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>47000</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>48000</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>49000</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>51000</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>53000</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>54000</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>55000</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>56000</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>"} , ignore_index=True)</t>
+  </si>
+  <si>
+    <t>" : "</t>
+  </si>
+  <si>
+    <t>" , update_name_col_1 : "</t>
+  </si>
+  <si>
+    <t>", update_name_col_3 : "</t>
+  </si>
+  <si>
+    <t>df_pres_result=df_pres_result.append({update_name_col_2 : "</t>
+  </si>
+  <si>
+    <t>", update_name_col_6 : "</t>
   </si>
 </sst>
 </file>
@@ -625,7 +1118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,6 +1141,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -681,7 +1181,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -707,6 +1207,10 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1750,7 +2254,7 @@
         <v>NET_MIG_</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="180" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1780,7 +2284,7 @@
         <v>NET_MIG_</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="195" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1810,7 +2314,7 @@
         <v>NET_MIG_</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" ht="195" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1840,7 +2344,7 @@
         <v>RESIDUAL_</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" ht="210" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1870,7 +2374,7 @@
         <v>RESIDUAL_</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" ht="210" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1900,7 +2404,7 @@
         <v>RESIDUAL_</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" ht="210" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1930,7 +2434,7 @@
         <v>RESIDUAL_</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" ht="225" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1960,7 +2464,7 @@
         <v>RESIDUAL_</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" ht="225" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1990,7 +2494,7 @@
         <v>GQ_ESTIMATES_</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" ht="240" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
@@ -3494,6 +3998,2509 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC803E9-11E1-48E6-B033-9C79842F9114}">
+  <dimension ref="A1:O54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="M54" sqref="M54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
+        <v>351</v>
+      </c>
+      <c r="O1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" t="str">
+        <f>$D$1&amp;B3&amp;$E$1&amp;A3&amp;$F$1&amp;C3&amp;$G$1&amp;C3&amp;$H$1</f>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "US" , update_name_col_1 : "00000", update_name_col_3 : "United States", update_name_col_6 : "United States"} , ignore_index=True)</v>
+      </c>
+      <c r="E3" t="str">
+        <f>$M$1&amp;C3&amp;$N$1&amp;B3&amp;$O$1</f>
+        <v xml:space="preserve">"United States" : "US", </v>
+      </c>
+      <c r="F3" t="str">
+        <f>E3</f>
+        <v xml:space="preserve">"United States" : "US", </v>
+      </c>
+      <c r="H3" t="str">
+        <f>$M$1&amp;A3&amp;$O$1</f>
+        <v xml:space="preserve">"00000", </v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:J3" si="0">$M$1&amp;B3&amp;$O$1</f>
+        <v xml:space="preserve">"US", </v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"United States", </v>
+      </c>
+      <c r="K3" t="str">
+        <f>H3</f>
+        <v xml:space="preserve">"00000", </v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:M3" si="1">I3</f>
+        <v xml:space="preserve">"US", </v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"United States", </v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D54" si="2">$D$1&amp;B4&amp;$E$1&amp;A4&amp;$F$1&amp;C4&amp;$G$1&amp;C4&amp;$H$1</f>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "AL" , update_name_col_1 : "01000", update_name_col_3 : "Alabama", update_name_col_6 : "Alabama"} , ignore_index=True)</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" ref="E4:E54" si="3">$M$1&amp;C4&amp;$N$1&amp;B4&amp;$O$1</f>
+        <v xml:space="preserve">"Alabama" : "AL", </v>
+      </c>
+      <c r="F4" t="str">
+        <f>F3&amp;E4</f>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", </v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H54" si="4">$M$1&amp;A4&amp;$O$1</f>
+        <v xml:space="preserve">"01000", </v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I54" si="5">$M$1&amp;B4&amp;$O$1</f>
+        <v xml:space="preserve">"AL", </v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J54" si="6">$M$1&amp;C4&amp;$O$1</f>
+        <v xml:space="preserve">"Alabama", </v>
+      </c>
+      <c r="K4" t="str">
+        <f>K3&amp;H4</f>
+        <v xml:space="preserve">"00000", "01000", </v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:M4" si="7">L3&amp;I4</f>
+        <v xml:space="preserve">"US", "AL", </v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">"United States", "Alabama", </v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "AK" , update_name_col_1 : "02000", update_name_col_3 : "Alaska", update_name_col_6 : "Alaska"} , ignore_index=True)</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Alaska" : "AK", </v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F54" si="8">F4&amp;E5</f>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", </v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"02000", </v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"AK", </v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Alaska", </v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5:K54" si="9">K4&amp;H5</f>
+        <v xml:space="preserve">"00000", "01000", "02000", </v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" ref="L5:L54" si="10">L4&amp;I5</f>
+        <v xml:space="preserve">"US", "AL", "AK", </v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ref="M5:M54" si="11">M4&amp;J5</f>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", </v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "AZ" , update_name_col_1 : "04000", update_name_col_3 : "Arizona", update_name_col_6 : "Arizona"} , ignore_index=True)</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Arizona" : "AZ", </v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", </v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"04000", </v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"AZ", </v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Arizona", </v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", </v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", </v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", </v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "AR" , update_name_col_1 : "05000", update_name_col_3 : "Arkansas", update_name_col_6 : "Arkansas"} , ignore_index=True)</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Arkansas" : "AR", </v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", </v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"05000", </v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"AR", </v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Arkansas", </v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", </v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", </v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", </v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "CA" , update_name_col_1 : "06000", update_name_col_3 : "California", update_name_col_6 : "California"} , ignore_index=True)</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"California" : "CA", </v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", </v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"06000", </v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"CA", </v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"California", </v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", </v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", </v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", </v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "CO" , update_name_col_1 : "08000", update_name_col_3 : "Colorado", update_name_col_6 : "Colorado"} , ignore_index=True)</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Colorado" : "CO", </v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", </v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"08000", </v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"CO", </v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Colorado", </v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", </v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", </v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", </v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "CT" , update_name_col_1 : "09000", update_name_col_3 : "Connecticut", update_name_col_6 : "Connecticut"} , ignore_index=True)</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Connecticut" : "CT", </v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", </v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"09000", </v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"CT", </v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Connecticut", </v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", </v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", </v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", </v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "DE" , update_name_col_1 : "10000", update_name_col_3 : "Delaware", update_name_col_6 : "Delaware"} , ignore_index=True)</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Delaware" : "DE", </v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", </v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"10000", </v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"DE", </v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Delaware", </v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", </v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", </v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", </v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "DC" , update_name_col_1 : "11000", update_name_col_3 : "District of Columbia", update_name_col_6 : "District of Columbia"} , ignore_index=True)</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"District of Columbia" : "DC", </v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", </v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"11000", </v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"DC", </v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"District of Columbia", </v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", </v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", </v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", </v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "FL" , update_name_col_1 : "12000", update_name_col_3 : "Florida", update_name_col_6 : "Florida"} , ignore_index=True)</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Florida" : "FL", </v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", </v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"12000", </v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"FL", </v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Florida", </v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", </v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", </v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", </v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "GA" , update_name_col_1 : "13000", update_name_col_3 : "Georgia", update_name_col_6 : "Georgia"} , ignore_index=True)</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Georgia" : "GA", </v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", </v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"13000", </v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"GA", </v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Georgia", </v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", </v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", </v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", </v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "HI" , update_name_col_1 : "15000", update_name_col_3 : "Hawaii", update_name_col_6 : "Hawaii"} , ignore_index=True)</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Hawaii" : "HI", </v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", </v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"15000", </v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"HI", </v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Hawaii", </v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", </v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", </v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", </v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "ID" , update_name_col_1 : "16000", update_name_col_3 : "Idaho", update_name_col_6 : "Idaho"} , ignore_index=True)</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Idaho" : "ID", </v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", </v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"16000", </v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"ID", </v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Idaho", </v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", </v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", </v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", </v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "IL" , update_name_col_1 : "17000", update_name_col_3 : "Illinois", update_name_col_6 : "Illinois"} , ignore_index=True)</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Illinois" : "IL", </v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", </v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"17000", </v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"IL", </v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Illinois", </v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", </v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", </v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", </v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C18" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "IN" , update_name_col_1 : "18000", update_name_col_3 : "Indiana", update_name_col_6 : "Indiana"} , ignore_index=True)</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Indiana" : "IN", </v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", </v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"18000", </v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"IN", </v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Indiana", </v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", </v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", </v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", </v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "IA" , update_name_col_1 : "19000", update_name_col_3 : "Iowa", update_name_col_6 : "Iowa"} , ignore_index=True)</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Iowa" : "IA", </v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", </v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"19000", </v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"IA", </v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Iowa", </v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", </v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", </v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", </v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "KS" , update_name_col_1 : "20000", update_name_col_3 : "Kansas", update_name_col_6 : "Kansas"} , ignore_index=True)</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Kansas" : "KS", </v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", </v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"20000", </v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"KS", </v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Kansas", </v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", </v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", </v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", </v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "KY" , update_name_col_1 : "21000", update_name_col_3 : "Kentucky", update_name_col_6 : "Kentucky"} , ignore_index=True)</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Kentucky" : "KY", </v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", </v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"21000", </v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"KY", </v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Kentucky", </v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", </v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", </v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", </v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "LA" , update_name_col_1 : "22000", update_name_col_3 : "Lousiana", update_name_col_6 : "Lousiana"} , ignore_index=True)</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Lousiana" : "LA", </v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", </v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"22000", </v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"LA", </v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Lousiana", </v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", </v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", </v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", </v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B23" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "ME" , update_name_col_1 : "23000", update_name_col_3 : "Maine", update_name_col_6 : "Maine"} , ignore_index=True)</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Maine" : "ME", </v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", </v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"23000", </v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"ME", </v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Maine", </v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", </v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", </v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", </v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B24" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "MD" , update_name_col_1 : "24000", update_name_col_3 : "Maryland", update_name_col_6 : "Maryland"} , ignore_index=True)</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Maryland" : "MD", </v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", </v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"24000", </v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"MD", </v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Maryland", </v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", </v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", </v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", </v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>260</v>
+      </c>
+      <c r="B25" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25" t="s">
+        <v>262</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "MA" , update_name_col_1 : "25000", update_name_col_3 : "Massachusetts", update_name_col_6 : "Massachusetts"} , ignore_index=True)</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Massachusetts" : "MA", </v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", </v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"25000", </v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"MA", </v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Massachusetts", </v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", </v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", </v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", </v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>263</v>
+      </c>
+      <c r="B26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "MI" , update_name_col_1 : "26000", update_name_col_3 : "Michigan", update_name_col_6 : "Michigan"} , ignore_index=True)</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Michigan" : "MI", </v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", </v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"26000", </v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"MI", </v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Michigan", </v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", </v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", </v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", </v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>266</v>
+      </c>
+      <c r="B27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C27" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "MN" , update_name_col_1 : "27000", update_name_col_3 : "Minnesota", update_name_col_6 : "Minnesota"} , ignore_index=True)</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Minnesota" : "MN", </v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", </v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"27000", </v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"MN", </v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Minnesota", </v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", </v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", </v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", </v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>269</v>
+      </c>
+      <c r="B28" t="s">
+        <v>270</v>
+      </c>
+      <c r="C28" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "MS" , update_name_col_1 : "28000", update_name_col_3 : "Mississippi", update_name_col_6 : "Mississippi"} , ignore_index=True)</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Mississippi" : "MS", </v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", </v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"28000", </v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"MS", </v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Mississippi", </v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", </v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", </v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", </v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>272</v>
+      </c>
+      <c r="B29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C29" t="s">
+        <v>274</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "MO" , update_name_col_1 : "29000", update_name_col_3 : "Missouri", update_name_col_6 : "Missouri"} , ignore_index=True)</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Missouri" : "MO", </v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", </v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"29000", </v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"MO", </v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Missouri", </v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", </v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", </v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", </v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>275</v>
+      </c>
+      <c r="B30" t="s">
+        <v>276</v>
+      </c>
+      <c r="C30" t="s">
+        <v>277</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "MT" , update_name_col_1 : "30000", update_name_col_3 : "Montana", update_name_col_6 : "Montana"} , ignore_index=True)</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Montana" : "MT", </v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", </v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"30000", </v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"MT", </v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Montana", </v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", </v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", </v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", </v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31" t="s">
+        <v>279</v>
+      </c>
+      <c r="C31" t="s">
+        <v>280</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "NE" , update_name_col_1 : "31000", update_name_col_3 : "Nebraska", update_name_col_6 : "Nebraska"} , ignore_index=True)</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Nebraska" : "NE", </v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", </v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"31000", </v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"NE", </v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Nebraska", </v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", </v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", </v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", </v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>281</v>
+      </c>
+      <c r="B32" t="s">
+        <v>282</v>
+      </c>
+      <c r="C32" t="s">
+        <v>283</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "NV" , update_name_col_1 : "32000", update_name_col_3 : "Nevada", update_name_col_6 : "Nevada"} , ignore_index=True)</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Nevada" : "NV", </v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", </v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"32000", </v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"NV", </v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Nevada", </v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", </v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", </v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", </v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33" t="s">
+        <v>285</v>
+      </c>
+      <c r="C33" t="s">
+        <v>286</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "NH" , update_name_col_1 : "33000", update_name_col_3 : "New Hampshire", update_name_col_6 : "New Hampshire"} , ignore_index=True)</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"New Hampshire" : "NH", </v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", </v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"33000", </v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"NH", </v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"New Hampshire", </v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", </v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", </v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", </v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" t="s">
+        <v>288</v>
+      </c>
+      <c r="C34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "NJ" , update_name_col_1 : "34000", update_name_col_3 : "New Jersey", update_name_col_6 : "New Jersey"} , ignore_index=True)</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"New Jersey" : "NJ", </v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", </v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"34000", </v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"NJ", </v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"New Jersey", </v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", </v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", </v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", </v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "NM" , update_name_col_1 : "35000", update_name_col_3 : "New Mexico", update_name_col_6 : "New Mexico"} , ignore_index=True)</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"New Mexico" : "NM", </v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", </v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"35000", </v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"NM", </v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"New Mexico", </v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", </v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", </v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", </v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B36" t="s">
+        <v>294</v>
+      </c>
+      <c r="C36" t="s">
+        <v>295</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "NY" , update_name_col_1 : "36000", update_name_col_3 : "New York", update_name_col_6 : "New York"} , ignore_index=True)</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"New York" : "NY", </v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", </v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"36000", </v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"NY", </v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"New York", </v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", </v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", </v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", </v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>296</v>
+      </c>
+      <c r="B37" t="s">
+        <v>297</v>
+      </c>
+      <c r="C37" t="s">
+        <v>298</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "NC" , update_name_col_1 : "37000", update_name_col_3 : "North Carolina", update_name_col_6 : "North Carolina"} , ignore_index=True)</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"North Carolina" : "NC", </v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", </v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"37000", </v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"NC", </v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"North Carolina", </v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", </v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", </v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", </v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>299</v>
+      </c>
+      <c r="B38" t="s">
+        <v>300</v>
+      </c>
+      <c r="C38" t="s">
+        <v>301</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "ND" , update_name_col_1 : "38000", update_name_col_3 : "North Dakota", update_name_col_6 : "North Dakota"} , ignore_index=True)</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"North Dakota" : "ND", </v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", </v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"38000", </v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"ND", </v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"North Dakota", </v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", </v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", </v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", </v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>302</v>
+      </c>
+      <c r="B39" t="s">
+        <v>303</v>
+      </c>
+      <c r="C39" t="s">
+        <v>304</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "OH" , update_name_col_1 : "39000", update_name_col_3 : "Ohio", update_name_col_6 : "Ohio"} , ignore_index=True)</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Ohio" : "OH", </v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", </v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"39000", </v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"OH", </v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Ohio", </v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", </v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", </v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", </v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B40" t="s">
+        <v>306</v>
+      </c>
+      <c r="C40" t="s">
+        <v>307</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "OK" , update_name_col_1 : "40000", update_name_col_3 : "Oklahoma", update_name_col_6 : "Oklahoma"} , ignore_index=True)</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Oklahoma" : "OK", </v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", </v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"40000", </v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"OK", </v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Oklahoma", </v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", </v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", </v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", </v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>308</v>
+      </c>
+      <c r="B41" t="s">
+        <v>309</v>
+      </c>
+      <c r="C41" t="s">
+        <v>310</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "OR" , update_name_col_1 : "41000", update_name_col_3 : "Oregon", update_name_col_6 : "Oregon"} , ignore_index=True)</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Oregon" : "OR", </v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", </v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"41000", </v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"OR", </v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Oregon", </v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", </v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", </v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", </v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>311</v>
+      </c>
+      <c r="B42" t="s">
+        <v>312</v>
+      </c>
+      <c r="C42" t="s">
+        <v>313</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "PA" , update_name_col_1 : "42000", update_name_col_3 : "Pennsylvania", update_name_col_6 : "Pennsylvania"} , ignore_index=True)</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Pennsylvania" : "PA", </v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", </v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"42000", </v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"PA", </v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Pennsylvania", </v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", </v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", </v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", </v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>314</v>
+      </c>
+      <c r="B43" t="s">
+        <v>315</v>
+      </c>
+      <c r="C43" t="s">
+        <v>316</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "RI" , update_name_col_1 : "44000", update_name_col_3 : "Rhode Island", update_name_col_6 : "Rhode Island"} , ignore_index=True)</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Rhode Island" : "RI", </v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", </v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"44000", </v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"RI", </v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Rhode Island", </v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", </v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", </v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", </v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>317</v>
+      </c>
+      <c r="B44" t="s">
+        <v>318</v>
+      </c>
+      <c r="C44" t="s">
+        <v>319</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "SC" , update_name_col_1 : "45000", update_name_col_3 : "South Carolina", update_name_col_6 : "South Carolina"} , ignore_index=True)</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"South Carolina" : "SC", </v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", </v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"45000", </v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"SC", </v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"South Carolina", </v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", </v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", </v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", </v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>320</v>
+      </c>
+      <c r="B45" t="s">
+        <v>321</v>
+      </c>
+      <c r="C45" t="s">
+        <v>322</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "SD" , update_name_col_1 : "46000", update_name_col_3 : "South Dakota", update_name_col_6 : "South Dakota"} , ignore_index=True)</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"South Dakota" : "SD", </v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", </v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"46000", </v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"SD", </v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"South Dakota", </v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", </v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", </v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", </v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>323</v>
+      </c>
+      <c r="B46" t="s">
+        <v>324</v>
+      </c>
+      <c r="C46" t="s">
+        <v>325</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "TN" , update_name_col_1 : "47000", update_name_col_3 : "Tennessee", update_name_col_6 : "Tennessee"} , ignore_index=True)</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Tennessee" : "TN", </v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", </v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"47000", </v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"TN", </v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Tennessee", </v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", </v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", </v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", </v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>326</v>
+      </c>
+      <c r="B47" t="s">
+        <v>327</v>
+      </c>
+      <c r="C47" t="s">
+        <v>328</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "TX" , update_name_col_1 : "48000", update_name_col_3 : "Texas", update_name_col_6 : "Texas"} , ignore_index=True)</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Texas" : "TX", </v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", </v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"48000", </v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"TX", </v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Texas", </v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", </v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", </v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", </v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>329</v>
+      </c>
+      <c r="B48" t="s">
+        <v>330</v>
+      </c>
+      <c r="C48" t="s">
+        <v>331</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "UT" , update_name_col_1 : "49000", update_name_col_3 : "Utah", update_name_col_6 : "Utah"} , ignore_index=True)</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Utah" : "UT", </v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", "Utah" : "UT", </v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"49000", </v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"UT", </v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Utah", </v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", "49000", </v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", "UT", </v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", "Utah", </v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>332</v>
+      </c>
+      <c r="B49" t="s">
+        <v>333</v>
+      </c>
+      <c r="C49" t="s">
+        <v>334</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "VT" , update_name_col_1 : "50000", update_name_col_3 : "Vermont", update_name_col_6 : "Vermont"} , ignore_index=True)</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Vermont" : "VT", </v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", "Utah" : "UT", "Vermont" : "VT", </v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"50000", </v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"VT", </v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Vermont", </v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", "49000", "50000", </v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", "UT", "VT", </v>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", "Utah", "Vermont", </v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>335</v>
+      </c>
+      <c r="B50" t="s">
+        <v>336</v>
+      </c>
+      <c r="C50" t="s">
+        <v>337</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "VA" , update_name_col_1 : "51000", update_name_col_3 : "Virginia", update_name_col_6 : "Virginia"} , ignore_index=True)</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Virginia" : "VA", </v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", "Utah" : "UT", "Vermont" : "VT", "Virginia" : "VA", </v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"51000", </v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"VA", </v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Virginia", </v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", "49000", "50000", "51000", </v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", "UT", "VT", "VA", </v>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", "Utah", "Vermont", "Virginia", </v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>338</v>
+      </c>
+      <c r="B51" t="s">
+        <v>339</v>
+      </c>
+      <c r="C51" t="s">
+        <v>340</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "WA" , update_name_col_1 : "53000", update_name_col_3 : "Washington", update_name_col_6 : "Washington"} , ignore_index=True)</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Washington" : "WA", </v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", "Utah" : "UT", "Vermont" : "VT", "Virginia" : "VA", "Washington" : "WA", </v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"53000", </v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"WA", </v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Washington", </v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", "49000", "50000", "51000", "53000", </v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", "UT", "VT", "VA", "WA", </v>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", "Utah", "Vermont", "Virginia", "Washington", </v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>341</v>
+      </c>
+      <c r="B52" t="s">
+        <v>342</v>
+      </c>
+      <c r="C52" t="s">
+        <v>343</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "WV" , update_name_col_1 : "54000", update_name_col_3 : "West Virginia", update_name_col_6 : "West Virginia"} , ignore_index=True)</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"West Virginia" : "WV", </v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", "Utah" : "UT", "Vermont" : "VT", "Virginia" : "VA", "Washington" : "WA", "West Virginia" : "WV", </v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"54000", </v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"WV", </v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"West Virginia", </v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", "49000", "50000", "51000", "53000", "54000", </v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", "UT", "VT", "VA", "WA", "WV", </v>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", "Utah", "Vermont", "Virginia", "Washington", "West Virginia", </v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>344</v>
+      </c>
+      <c r="B53" t="s">
+        <v>345</v>
+      </c>
+      <c r="C53" t="s">
+        <v>346</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "WI" , update_name_col_1 : "55000", update_name_col_3 : "Wisconsin", update_name_col_6 : "Wisconsin"} , ignore_index=True)</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Wisconsin" : "WI", </v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", "Utah" : "UT", "Vermont" : "VT", "Virginia" : "VA", "Washington" : "WA", "West Virginia" : "WV", "Wisconsin" : "WI", </v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"55000", </v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"WI", </v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Wisconsin", </v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", "49000", "50000", "51000", "53000", "54000", "55000", </v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", "UT", "VT", "VA", "WA", "WV", "WI", </v>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", "Utah", "Vermont", "Virginia", "Washington", "West Virginia", "Wisconsin", </v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>347</v>
+      </c>
+      <c r="B54" t="s">
+        <v>348</v>
+      </c>
+      <c r="C54" t="s">
+        <v>349</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="2"/>
+        <v>df_pres_result=df_pres_result.append({update_name_col_2 : "WY" , update_name_col_1 : "56000", update_name_col_3 : "Wyoming", update_name_col_6 : "Wyoming"} , ignore_index=True)</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"Wyoming" : "WY", </v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">"United States" : "US", "Alabama" : "AL", "Alaska" : "AK", "Arizona" : "AZ", "Arkansas" : "AR", "California" : "CA", "Colorado" : "CO", "Connecticut" : "CT", "Delaware" : "DE", "District of Columbia" : "DC", "Florida" : "FL", "Georgia" : "GA", "Hawaii" : "HI", "Idaho" : "ID", "Illinois" : "IL", "Indiana" : "IN", "Iowa" : "IA", "Kansas" : "KS", "Kentucky" : "KY", "Lousiana" : "LA", "Maine" : "ME", "Maryland" : "MD", "Massachusetts" : "MA", "Michigan" : "MI", "Minnesota" : "MN", "Mississippi" : "MS", "Missouri" : "MO", "Montana" : "MT", "Nebraska" : "NE", "Nevada" : "NV", "New Hampshire" : "NH", "New Jersey" : "NJ", "New Mexico" : "NM", "New York" : "NY", "North Carolina" : "NC", "North Dakota" : "ND", "Ohio" : "OH", "Oklahoma" : "OK", "Oregon" : "OR", "Pennsylvania" : "PA", "Rhode Island" : "RI", "South Carolina" : "SC", "South Dakota" : "SD", "Tennessee" : "TN", "Texas" : "TX", "Utah" : "UT", "Vermont" : "VT", "Virginia" : "VA", "Washington" : "WA", "West Virginia" : "WV", "Wisconsin" : "WI", "Wyoming" : "WY", </v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">"56000", </v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"WY", </v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"Wyoming", </v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">"00000", "01000", "02000", "04000", "05000", "06000", "08000", "09000", "10000", "11000", "12000", "13000", "15000", "16000", "17000", "18000", "19000", "20000", "21000", "22000", "23000", "24000", "25000", "26000", "27000", "28000", "29000", "30000", "31000", "32000", "33000", "34000", "35000", "36000", "37000", "38000", "39000", "40000", "41000", "42000", "44000", "45000", "46000", "47000", "48000", "49000", "50000", "51000", "53000", "54000", "55000", "56000", </v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">"US", "AL", "AK", "AZ", "AR", "CA", "CO", "CT", "DE", "DC", "FL", "GA", "HI", "ID", "IL", "IN", "IA", "KS", "KY", "LA", "ME", "MD", "MA", "MI", "MN", "MS", "MO", "MT", "NE", "NV", "NH", "NJ", "NM", "NY", "NC", "ND", "OH", "OK", "OR", "PA", "RI", "SC", "SD", "TN", "TX", "UT", "VT", "VA", "WA", "WV", "WI", "WY", </v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">"United States", "Alabama", "Alaska", "Arizona", "Arkansas", "California", "Colorado", "Connecticut", "Delaware", "District of Columbia", "Florida", "Georgia", "Hawaii", "Idaho", "Illinois", "Indiana", "Iowa", "Kansas", "Kentucky", "Lousiana", "Maine", "Maryland", "Massachusetts", "Michigan", "Minnesota", "Mississippi", "Missouri", "Montana", "Nebraska", "Nevada", "New Hampshire", "New Jersey", "New Mexico", "New York", "North Carolina", "North Dakota", "Ohio", "Oklahoma", "Oregon", "Pennsylvania", "Rhode Island", "South Carolina", "South Dakota", "Tennessee", "Texas", "Utah", "Vermont", "Virginia", "Washington", "West Virginia", "Wisconsin", "Wyoming", </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AF7F3D-DB5A-4EEC-AF76-0F72C2CC8DE5}">
   <dimension ref="B1:E28"/>
   <sheetViews>
@@ -3952,11 +6959,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2951A278-933A-4946-A041-108F921DDC3D}">
   <dimension ref="A2:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>